<commit_message>
fix po deliverables for sprint 7
Co-authored-by: LeaBuchner <lea.buchner@proton.me>
Signed-off-by: engelharddirk <dirk.engelhard@hotmail.de>
</commit_message>
<xml_diff>
--- a/Deliverables/sprint-07/planning-documents.xlsx
+++ b/Deliverables/sprint-07/planning-documents.xlsx
@@ -2922,8 +2922,8 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1639752183"/>
-        <c:axId val="697202122"/>
+        <c:axId val="772928854"/>
+        <c:axId val="1042882111"/>
       </c:barChart>
       <c:lineChart>
         <c:varyColors val="0"/>
@@ -2962,11 +2962,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1639752183"/>
-        <c:axId val="697202122"/>
+        <c:axId val="772928854"/>
+        <c:axId val="1042882111"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1639752183"/>
+        <c:axId val="772928854"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3018,10 +3018,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="697202122"/>
+        <c:crossAx val="1042882111"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="697202122"/>
+        <c:axId val="1042882111"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3096,7 +3096,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1639752183"/>
+        <c:crossAx val="772928854"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3250,11 +3250,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1904897826"/>
-        <c:axId val="947737003"/>
+        <c:axId val="934284233"/>
+        <c:axId val="262814088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1904897826"/>
+        <c:axId val="934284233"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3306,10 +3306,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="947737003"/>
+        <c:crossAx val="262814088"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="947737003"/>
+        <c:axId val="262814088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3384,7 +3384,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1904897826"/>
+        <c:crossAx val="934284233"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3538,11 +3538,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1582393933"/>
-        <c:axId val="1121772805"/>
+        <c:axId val="1454159181"/>
+        <c:axId val="1195998882"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1582393933"/>
+        <c:axId val="1454159181"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3594,10 +3594,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1121772805"/>
+        <c:crossAx val="1195998882"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1121772805"/>
+        <c:axId val="1195998882"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3672,7 +3672,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1582393933"/>
+        <c:crossAx val="1454159181"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5283,7 +5283,7 @@
       </c>
       <c r="B23" s="68">
         <f>'Velocity Tracking'!C2</f>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
       <c r="C23" s="64" t="s">
         <v>230</v>
@@ -14945,7 +14945,7 @@
       </c>
       <c r="B23" s="68">
         <f>'Velocity Tracking'!C2</f>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
       <c r="C23" s="64" t="s">
         <v>230</v>
@@ -19058,7 +19058,7 @@
       </c>
       <c r="C2" s="66">
         <f t="shared" ref="C2:C16" si="1">AVERAGE($B$2:$B$16)</f>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="3">
@@ -19072,7 +19072,7 @@
       </c>
       <c r="C3" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="4">
@@ -19086,7 +19086,7 @@
       </c>
       <c r="C4" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="5">
@@ -19100,7 +19100,7 @@
       </c>
       <c r="C5" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="6">
@@ -19114,7 +19114,7 @@
       </c>
       <c r="C6" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="7">
@@ -19128,7 +19128,7 @@
       </c>
       <c r="C7" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="8">
@@ -19136,10 +19136,13 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="12">
+        <f>'Final Project Release plan'!F9</f>
+        <v>25</v>
+      </c>
       <c r="C8" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="9">
@@ -19150,7 +19153,7 @@
       <c r="B9" s="12"/>
       <c r="C9" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="10">
@@ -19161,7 +19164,7 @@
       <c r="B10" s="12"/>
       <c r="C10" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="11">
@@ -19175,7 +19178,7 @@
       </c>
       <c r="C11" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="12">
@@ -19189,7 +19192,7 @@
       </c>
       <c r="C12" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="13">
@@ -19203,7 +19206,7 @@
       </c>
       <c r="C13" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="14">
@@ -19217,7 +19220,7 @@
       </c>
       <c r="C14" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="15">
@@ -19231,7 +19234,7 @@
       </c>
       <c r="C15" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="16">
@@ -19242,7 +19245,7 @@
       <c r="B16" s="2"/>
       <c r="C16" s="66">
         <f t="shared" si="1"/>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
     </row>
     <row r="17">
@@ -19298,7 +19301,7 @@
       </c>
       <c r="B23" s="68">
         <f>'Velocity Tracking'!C2</f>
-        <v>17.83333333</v>
+        <v>18.85714286</v>
       </c>
       <c r="C23" s="64" t="s">
         <v>230</v>

</xml_diff>